<commit_message>
Update IP - EX 30 - Remover duplicatas (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 30 - Remover duplicatas (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 30 - Remover duplicatas (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825E2E53-E057-43B5-954F-7EA82E049D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418EB88C-B89D-4C5D-9F68-ECBF6406113A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>NOMES</t>
   </si>
@@ -301,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -556,36 +578,6 @@
       <right style="dotted">
         <color theme="1" tint="0.499984740745262"/>
       </right>
-      <top style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
       <top/>
       <bottom style="dotted">
         <color theme="1" tint="0.499984740745262"/>
@@ -719,21 +711,6 @@
         <color theme="1" tint="0.499984740745262"/>
       </top>
       <bottom style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="medium">
         <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -749,7 +726,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,52 +765,43 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="34" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="32" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1606,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1616,96 +1584,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="46"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="49"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="49"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1795,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q87"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,457 +1782,567 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="str">
+      <c r="B2" s="41" t="str">
         <f>CONTEÚDO!B2</f>
         <v>Remover Duplicatas</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="46"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="49"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="49"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="J8" s="25" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="J8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="2:17" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="21" t="s">
         <v>10</v>
       </c>
+      <c r="J10" t="str" cm="1">
+        <f t="array" ref="J10:K39">_xlfn.UNIQUE(E10:F39)</f>
+        <v>NOMES</v>
+      </c>
+      <c r="K10" t="str">
+        <v>VALORES</v>
+      </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="19">
         <v>87</v>
       </c>
+      <c r="J11" t="str">
+        <v>MARIA</v>
+      </c>
+      <c r="K11">
+        <v>87</v>
+      </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17">
+        <v>154</v>
+      </c>
+      <c r="J12" t="str">
+        <v>JOÃO</v>
+      </c>
+      <c r="K12">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="17">
+        <v>36</v>
+      </c>
+      <c r="J13" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="F14" s="17">
+        <v>42</v>
+      </c>
+      <c r="J14" t="str">
+        <v>MARIA</v>
+      </c>
+      <c r="K14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="17">
+        <v>44</v>
+      </c>
+      <c r="J15" t="str">
+        <v>CAMILA</v>
+      </c>
+      <c r="K15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="17">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="17">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="F16" s="17">
+        <v>168</v>
+      </c>
+      <c r="J16" t="str">
+        <v>MARIA</v>
+      </c>
+      <c r="K16">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="17">
+        <v>158</v>
+      </c>
+      <c r="J17" t="str">
+        <v>JOAQUIM</v>
+      </c>
+      <c r="K17">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="17">
+        <v>64</v>
+      </c>
+      <c r="J18" t="str">
+        <v>GUSTAVO</v>
+      </c>
+      <c r="K18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F19" s="17">
+        <v>116</v>
+      </c>
+      <c r="J19" t="str">
+        <v>MARIA</v>
+      </c>
+      <c r="K19">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="17">
+        <v>129</v>
+      </c>
+      <c r="J20" t="str">
+        <v>JOAQUIM</v>
+      </c>
+      <c r="K20">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="17">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="17">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="17">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="F21" s="17">
+        <v>159</v>
+      </c>
+      <c r="J21" t="str">
+        <v>MARIA</v>
+      </c>
+      <c r="K21">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="17">
+        <v>150</v>
+      </c>
+      <c r="J22" t="str">
+        <v>JOSÉ</v>
+      </c>
+      <c r="K22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="17">
+        <v>81</v>
+      </c>
+      <c r="J23" t="str">
+        <v>LUCAS</v>
+      </c>
+      <c r="K23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="17">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+      <c r="F24" s="17">
+        <v>100</v>
+      </c>
+      <c r="J24" t="str">
+        <v>JOAQUIM</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="17">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="17">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="17">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="17">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="17">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>5</v>
-      </c>
       <c r="F25" s="17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
-        <v>6</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="J25" t="str">
+        <v>GUSTAVO</v>
+      </c>
+      <c r="K25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E26" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="17">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
-        <v>6</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="J26" t="str">
+        <v>GUSTAVO</v>
+      </c>
+      <c r="K26">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E27" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F27" s="17">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" t="str">
+        <v>JOSÉ</v>
+      </c>
+      <c r="K27">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="17">
+        <v>38</v>
+      </c>
+      <c r="J28" t="str">
+        <v>JOAQUIM</v>
+      </c>
+      <c r="K28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="17">
+        <v>136</v>
+      </c>
+      <c r="J29" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K29">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="F30" s="17">
+        <v>21</v>
+      </c>
+      <c r="J30" t="str">
+        <v>JOSÉ</v>
+      </c>
+      <c r="K30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="17">
+        <v>174</v>
+      </c>
+      <c r="J31" t="str">
+        <v>FERNANDO</v>
+      </c>
+      <c r="K31">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17">
+        <v>106</v>
+      </c>
+      <c r="J32" t="str">
+        <v>JOÃO</v>
+      </c>
+      <c r="K32">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E33" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="F33" s="17">
+        <v>128</v>
+      </c>
+      <c r="J33" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K33">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E34" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="17">
+        <v>112</v>
+      </c>
+      <c r="J34" t="str">
+        <v>JOÃO</v>
+      </c>
+      <c r="K34">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E35" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="17">
+        <v>144</v>
+      </c>
+      <c r="J35" t="str">
+        <v>FERNANDO</v>
+      </c>
+      <c r="K35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E36" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="17">
+        <v>145</v>
+      </c>
+      <c r="J36" t="str">
+        <v>CAMILA</v>
+      </c>
+      <c r="K36">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E37" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="17">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="17">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="17">
+      <c r="F37" s="17">
         <v>106</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="17">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="17">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="17">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="17">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="J37" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K37">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="17">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="28" t="s">
-        <v>8</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="J38" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K38">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="17">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" s="19">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="J39" t="str">
+        <v>RAFAELA</v>
+      </c>
+      <c r="K39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" ht="3.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="5:11" ht="3.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="5:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2294,98 +2372,98 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="37"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="37"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="37"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="37"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="2:6" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="37"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="33"/>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>